<commit_message>
Update Projecttaken persoonlijke ontwikkeling.xlsx with recent changes
</commit_message>
<xml_diff>
--- a/Projecttaken persoonlijke ontwikkeling.xlsx
+++ b/Projecttaken persoonlijke ontwikkeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rinse\source\repos\Zaibatsu89\Website-Ontspanning-Door-Inspanning\xs4all\jobflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD85F8B7-46B8-4D9E-BC1E-EEE6166EBA89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902BE986-D909-4BAF-BB19-A76BCB7C9390}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>Taak</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>"Heb ik alle vinkjes volgens de checklist van de analyse afgevinkt?" in analyse flowchart, i.p.v. "Conclusie: ..."</t>
+  </si>
+  <si>
+    <t>"Start Tijdsregistratie (in Jira)" en "Ga naar Analyse" vervangen door "Bevindingen delen" in intake flowchart</t>
+  </si>
+  <si>
+    <t>Voeg "Jira-status OK?" en "Duidelijke beschrijving? (100% compleet en gevalideerd)" of "Meld probleem" toe na "Issue ontvangen" in intake flowchart</t>
+  </si>
+  <si>
+    <t>Voeg "Start timer 5 m." toe na "Issue ontvangen" in intake flowchart</t>
   </si>
 </sst>
 </file>
@@ -146,7 +155,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-m\-yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -188,6 +197,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -197,7 +221,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -385,11 +409,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF374139"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF374139"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -480,6 +522,24 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -544,7 +604,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Taken" displayName="Taken" ref="A1:I24" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Taken" displayName="Taken" ref="A1:I27" headerRowDxfId="0">
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Taak"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prioriteit"/>
@@ -761,7 +821,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -781,7 +841,7 @@
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -810,400 +870,470 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="11">
+        <v>45826</v>
+      </c>
+      <c r="F2" s="11">
+        <v>45826</v>
+      </c>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="31">
+        <v>45826</v>
+      </c>
+      <c r="F3" s="31">
+        <v>45826</v>
+      </c>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="31">
+        <v>45826</v>
+      </c>
+      <c r="F4" s="31">
+        <v>45826</v>
+      </c>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="33"/>
+    </row>
+    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E5" s="5">
         <v>45821</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F5" s="5">
         <v>45828</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E6" s="11">
         <v>45821</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F6" s="11">
         <v>45828</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E7" s="5">
         <v>45821</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F7" s="5">
         <v>45828</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="13"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="13"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="13"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="13"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="13"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="13"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B24" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C24" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D24" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E24" s="11">
         <v>45814</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F24" s="11">
         <v>45821</v>
       </c>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="13"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="13"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E25" s="5">
         <v>45814</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F25" s="5">
         <v>45821</v>
       </c>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B26" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C26" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D26" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E26" s="11">
         <v>45814</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F26" s="11">
         <v>45821</v>
       </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="13"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="13"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B27" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C27" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="D27" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E27" s="25">
         <v>45814</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F27" s="25">
         <v>45821</v>
       </c>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="27"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="27"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="D2:D24" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A5:A27 I2:I27 G2:G27" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation type="list" allowBlank="1" sqref="D2:D27" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Nog niet gestart,In behandeling,Geblokkeerd,Afgerond"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:F24" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:F27" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>OR(NOT(ISERROR(DATEVALUE(E2))), AND(ISNUMBER(E2), LEFT(CELL("format", E2))="D"))</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:A24 G2:G24 I2:I24" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation type="list" allowBlank="1" sqref="B2:B24" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B2:B27" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"P0,P1,P2,P3"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C21" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C22" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C23" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C24" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C24" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C25" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C26" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C27" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>